<commit_message>
add admin to database
</commit_message>
<xml_diff>
--- a/datafiles/game.xlsx
+++ b/datafiles/game.xlsx
@@ -418,7 +418,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -470,7 +470,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="3">
-        <v>41983</v>
+        <v>41924</v>
       </c>
     </row>
   </sheetData>

</xml_diff>